<commit_message>
feat: basci tags system with strings
</commit_message>
<xml_diff>
--- a/Python/20210915_steamlit_video_bookmarks/modified.xlsx
+++ b/Python/20210915_steamlit_video_bookmarks/modified.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>FilePath</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -496,6 +501,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\不僅僅是編程｜如何成為成功的工程師 6-39 screenshot.png</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['b', 'c']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,6 +538,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\不僅僅是編程｜如何成為成功的工程師 7-17 screenshot.png</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['g', 'a']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,6 +575,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\不僅僅是編程｜如何成為成功的工程師 7-19 screenshot.png</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['b', 'a']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -592,6 +612,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\不僅僅是編程｜如何成為成功的工程師 7-22 screenshot.png</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['g', 'b']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -624,6 +649,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\好和弦教你做 8-bit 音樂！懷舊電玩風～ 2-44 screenshot.png</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['c', 'b']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -656,6 +686,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\好和弦教你做 8-bit 音樂！懷舊電玩風～ 5-7 screenshot.png</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['c', 'f']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -688,6 +723,11 @@
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\超簡單又厲害的編曲軟體 - PixiTracker！ 10-2 screenshot.png</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>a, c, b</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -718,6 +758,11 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>g:\my_coding\Python\20210915_steamlit_video_bookmarks\res\超簡單又厲害的編曲軟體 - PixiTracker！ 10-4 screenshot.png</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['e', 'c']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: more searchYT and check videoname
</commit_message>
<xml_diff>
--- a/Python/20210915_steamlit_video_bookmarks/modified.xlsx
+++ b/Python/20210915_steamlit_video_bookmarks/modified.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,21 @@
           <t>LinkCK</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Channel</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,12 +528,27 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>a, b</t>
+          <t>職場</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>0</v>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>7:51</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>xS5Lv7-bMYI</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>HackBear 泰瑞</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -554,12 +584,27 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>職場</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>0</v>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>7:51</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>xS5Lv7-bMYI</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>HackBear 泰瑞</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -595,12 +640,27 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>d, b</t>
+          <t>職場</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>0</v>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>7:51</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>xS5Lv7-bMYI</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>HackBear 泰瑞</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -636,12 +696,27 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>c, c</t>
+          <t>職場</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>0</v>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>7:51</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>xS5Lv7-bMYI</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>HackBear 泰瑞</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -677,12 +752,27 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>d, c</t>
+          <t>編曲</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>0</v>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>8TbGCGDEgFk</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>NiceChord (好和弦)</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -718,12 +808,27 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>編曲</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
-        <v>0</v>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>11:29</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>8TbGCGDEgFk</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>NiceChord (好和弦)</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -759,12 +864,27 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>c, c</t>
+          <t>編曲</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>0</v>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>11:08</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>hciSF-wGlyc</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>NiceChord (好和弦)</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -800,12 +920,27 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>d, c</t>
+          <t>編曲</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
-        <v>0</v>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>11:08</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>hciSF-wGlyc</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>NiceChord (好和弦)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>